<commit_message>
Fixed Print Area and Settings for the new report layout
</commit_message>
<xml_diff>
--- a/templates/Template Sheets.xlsx
+++ b/templates/Template Sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Twitch-TikTok-Discord-Queue-Bot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159A67F-418C-4E35-8063-BB6D74BB5B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2063843-38BE-4A2B-AA85-F7774BF40F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6122,7 +6122,7 @@
   <dimension ref="A2:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6369,7 +6369,7 @@
       <formula>$F$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed sum formula in template
</commit_message>
<xml_diff>
--- a/templates/Template Sheets.xlsx
+++ b/templates/Template Sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Twitch-TikTok-Discord-Queue-Bot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2063843-38BE-4A2B-AA85-F7774BF40F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070A51DB-4619-4596-9A75-B45C7C544A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -516,7 +516,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -553,6 +552,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,8 +804,8 @@
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C3" s="13" t="s">
@@ -817,11 +817,11 @@
       <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="43">
         <f ca="1">TODAY()</f>
         <v>45841</v>
       </c>
-      <c r="I3" s="43"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
@@ -833,11 +833,11 @@
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
     </row>
     <row r="5" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C5" s="13" t="s">
@@ -861,9 +861,9 @@
       <c r="H7" s="12"/>
       <c r="I7" s="7"/>
       <c r="J7" s="12"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H8" s="12"/>
@@ -6122,7 +6122,7 @@
   <dimension ref="A2:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6147,38 +6147,38 @@
     </row>
     <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26"/>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26"/>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="38" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="28"/>
@@ -6198,11 +6198,11 @@
         <v>0</v>
       </c>
       <c r="E5" s="20">
-        <f>SUM(Q:Q)</f>
+        <f>SUM(N:N)</f>
         <v>0</v>
       </c>
       <c r="F5" s="20">
-        <f>SUM(S:S)</f>
+        <f>SUM(P:P)</f>
         <v>0</v>
       </c>
       <c r="G5" s="28"/>
@@ -6212,7 +6212,7 @@
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="31">
+      <c r="F6" s="45">
         <f>SUM(B5:E5)</f>
         <v>0</v>
       </c>
@@ -6241,22 +6241,22 @@
       <c r="D13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="32"/>
       <c r="K13" s="30"/>
-      <c r="L13" s="33"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="33"/>
+      <c r="N13" s="32"/>
       <c r="O13" s="30"/>
-      <c r="P13" s="33"/>
+      <c r="P13" s="32"/>
       <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="I14" s="31"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D15" s="19" t="s">
@@ -6274,91 +6274,91 @@
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I19" s="33"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.2">
       <c r="J20" s="30"/>
     </row>
     <row r="22" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="H22" s="32"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="22"/>
-      <c r="J22" s="33"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="30"/>
-      <c r="L22" s="33"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="30"/>
-      <c r="N22" s="33"/>
+      <c r="N22" s="32"/>
       <c r="O22" s="30"/>
-      <c r="P22" s="33"/>
+      <c r="P22" s="32"/>
       <c r="Q22" s="30"/>
     </row>
     <row r="23" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I23" s="32"/>
+      <c r="I23" s="31"/>
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I28" s="33"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="4:17" x14ac:dyDescent="0.2">
       <c r="J29" s="30"/>
     </row>
     <row r="31" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="H31" s="32"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="22"/>
-      <c r="J31" s="33"/>
+      <c r="J31" s="32"/>
       <c r="K31" s="30"/>
-      <c r="L31" s="33"/>
+      <c r="L31" s="32"/>
       <c r="M31" s="30"/>
-      <c r="N31" s="33"/>
+      <c r="N31" s="32"/>
       <c r="O31" s="30"/>
-      <c r="P31" s="33"/>
+      <c r="P31" s="32"/>
       <c r="Q31" s="30"/>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I32" s="32"/>
+      <c r="I32" s="31"/>
     </row>
     <row r="37" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="I37" s="33"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J38" s="30"/>
     </row>
     <row r="40" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H40" s="32"/>
+      <c r="H40" s="31"/>
       <c r="I40" s="22"/>
-      <c r="J40" s="33"/>
+      <c r="J40" s="32"/>
       <c r="K40" s="30"/>
-      <c r="L40" s="33"/>
+      <c r="L40" s="32"/>
       <c r="M40" s="30"/>
-      <c r="N40" s="33"/>
+      <c r="N40" s="32"/>
       <c r="O40" s="30"/>
-      <c r="P40" s="33"/>
+      <c r="P40" s="32"/>
       <c r="Q40" s="30"/>
     </row>
     <row r="41" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="I41" s="32"/>
+      <c r="I41" s="31"/>
     </row>
     <row r="46" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="I46" s="33"/>
+      <c r="I46" s="32"/>
     </row>
     <row r="47" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J47" s="30"/>
     </row>
     <row r="49" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="H49" s="32"/>
+      <c r="H49" s="31"/>
       <c r="I49" s="22"/>
-      <c r="J49" s="33"/>
+      <c r="J49" s="32"/>
       <c r="K49" s="30"/>
-      <c r="L49" s="33"/>
+      <c r="L49" s="32"/>
       <c r="M49" s="30"/>
-      <c r="N49" s="33"/>
+      <c r="N49" s="32"/>
       <c r="O49" s="30"/>
-      <c r="P49" s="33"/>
+      <c r="P49" s="32"/>
       <c r="Q49" s="30"/>
     </row>
     <row r="50" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="I50" s="32"/>
+      <c r="I50" s="31"/>
     </row>
     <row r="55" spans="8:17" x14ac:dyDescent="0.2">
-      <c r="I55" s="33"/>
+      <c r="I55" s="32"/>
     </row>
     <row r="56" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J56" s="30"/>

</xml_diff>